<commit_message>
corrected rule number for 32274
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-microsoft-windows-2012r2-member-server-stig-overlay.xlsx
+++ b/cms-ars-3.1-high-microsoft-windows-2012r2-member-server-stig-overlay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ADBD1733-99FB-49EC-869B-B6F51A80185C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D392C5-E955-4F09-A87F-57E1C35A4BDC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="W2012r2MS" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4840" uniqueCount="2851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4840" uniqueCount="2852">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -14129,6 +14129,9 @@
       <t xml:space="preserve">
 Std.1 - Perform full backups weekly to separate media. Perform incremental or differential backups daily to separate media.  Backups to include user-level and system-level information (including system state information).  Three (3) generations of backups (full plus all related incremental or differential backups) are stored off-site.  Off-site and on-site backups must be logged with name, date, time, and action.Std.2 - Backups must be compliant with CMS requirements for protecting data at rest. (see SC-28)</t>
     </r>
+  </si>
+  <si>
+    <t>V-32274</t>
   </si>
 </sst>
 </file>
@@ -14786,7 +14789,16 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -15102,7 +15114,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -30293,7 +30305,7 @@
     </row>
     <row r="252" spans="1:27" ht="409.6">
       <c r="A252" s="1" t="s">
-        <v>1934</v>
+        <v>2851</v>
       </c>
       <c r="B252" s="5" t="s">
         <v>24</v>
@@ -35662,7 +35674,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA339" xr:uid="{D34002B2-9078-4272-8ECD-741DADBB6AEE}"/>
+  <autoFilter ref="A1:AA339" xr:uid="{D34002B2-9078-4272-8ECD-741DADBB6AEE}">
+    <sortState ref="A292:AA292">
+      <sortCondition sortBy="cellColor" ref="A1:A339" dxfId="0"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>